<commit_message>
memperbaiki tabel harga, deskripsi dan stok
</commit_message>
<xml_diff>
--- a/public/template-data.xlsx
+++ b/public/template-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gudang-farmasi-drug\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE39F51C-C54B-4C59-9F83-7489267DF4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982CDD0D-7ECB-4BE1-A7FE-E41455312F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="2420" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Metode Pembayaran</t>
+  </si>
+  <si>
+    <t>Deskripsi</t>
+  </si>
+  <si>
+    <t>Stok</t>
   </si>
 </sst>
 </file>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,7 +449,7 @@
     <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,8 +477,14 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -482,8 +494,10 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -493,8 +507,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -504,6 +520,8 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
supplier download, delete metode and stok, and skip impor for name same, and to error validation
</commit_message>
<xml_diff>
--- a/public/template-data.xlsx
+++ b/public/template-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gudang-farmasi-drug\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982CDD0D-7ECB-4BE1-A7FE-E41455312F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF89C92-591A-416F-A8E8-3AAFEA9B25E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="2420" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>No</t>
   </si>
@@ -56,21 +56,12 @@
   <si>
     <t>Satuan Besar</t>
   </si>
-  <si>
-    <t>Metode Pembayaran</t>
-  </si>
-  <si>
-    <t>Deskripsi</t>
-  </si>
-  <si>
-    <t>Stok</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -82,6 +73,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -429,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,11 +440,11 @@
     <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="64.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" customWidth="1"/>
     <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,17 +469,8 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -493,11 +479,8 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -506,11 +489,8 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -519,11 +499,269 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>